<commit_message>
working on housework edits
</commit_message>
<xml_diff>
--- a/work/BicarbSoda/sodiumbicarbonate.xlsx
+++ b/work/BicarbSoda/sodiumbicarbonate.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26124"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Cat/Documents/PhD/work/BicarbSoda/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="10940" yWindow="-80" windowWidth="21120" windowHeight="13800" tabRatio="500"/>
+    <workbookView xWindow="7680" yWindow="460" windowWidth="21120" windowHeight="13800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
@@ -480,8 +485,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Verdana"/>
@@ -526,7 +531,12 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -849,27 +859,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr published="0" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="D50" sqref="D50"/>
+    <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>99</v>
       </c>
@@ -883,7 +893,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>105</v>
       </c>
@@ -900,7 +910,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>109</v>
       </c>
@@ -917,7 +927,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
         <v>112</v>
       </c>
@@ -934,7 +944,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
         <v>113</v>
       </c>
@@ -951,7 +961,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>97</v>
       </c>
@@ -968,7 +978,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>98</v>
       </c>
@@ -985,7 +995,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -1002,7 +1012,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -1019,7 +1029,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -1036,7 +1046,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>69</v>
       </c>
@@ -1053,7 +1063,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
         <v>72</v>
       </c>
@@ -1073,7 +1083,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -1090,7 +1100,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:6">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
         <v>79</v>
       </c>
@@ -1107,7 +1117,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
         <v>83</v>
       </c>
@@ -1127,7 +1137,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A18" t="s">
         <v>51</v>
       </c>
@@ -1144,7 +1154,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1161,7 +1171,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="20" spans="1:6">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -1178,7 +1188,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
         <v>56</v>
       </c>
@@ -1195,7 +1205,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>61</v>
       </c>
@@ -1215,7 +1225,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1232,7 +1242,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
         <v>66</v>
       </c>
@@ -1249,7 +1259,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -1266,7 +1276,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A26" t="s">
         <v>41</v>
       </c>
@@ -1283,7 +1293,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A27" t="s">
         <v>45</v>
       </c>
@@ -1300,7 +1310,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A28" t="s">
         <v>48</v>
       </c>
@@ -1317,7 +1327,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="1:6">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A29" t="s">
         <v>50</v>
       </c>
@@ -1334,7 +1344,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="1:6">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1354,7 +1364,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:6">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1371,7 +1381,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="32" spans="1:6">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1388,7 +1398,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>36</v>
       </c>
@@ -1405,7 +1415,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A34" t="s">
         <v>37</v>
       </c>
@@ -1422,7 +1432,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="35" spans="1:5">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>76</v>
       </c>
@@ -1439,7 +1449,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="36" spans="1:5">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>24</v>
       </c>
@@ -1456,7 +1466,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="16">
+    <row r="39" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="C39" t="s">
         <v>11</v>
       </c>
@@ -1465,7 +1475,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="16">
+    <row r="40" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="C40" t="s">
         <v>15</v>
       </c>
@@ -1474,7 +1484,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="16">
+    <row r="41" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="C41" t="s">
         <v>16</v>
       </c>
@@ -1483,7 +1493,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="16">
+    <row r="42" spans="1:5" ht="17" x14ac:dyDescent="0.2">
       <c r="C42" t="s">
         <v>17</v>
       </c>
@@ -1492,7 +1502,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="43" spans="1:5">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C43" t="s">
         <v>19</v>
       </c>
@@ -1501,7 +1511,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:5">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C44" t="s">
         <v>20</v>
       </c>
@@ -1510,7 +1520,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:5">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C45" t="s">
         <v>0</v>
       </c>
@@ -1519,7 +1529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:5">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C46" t="s">
         <v>1</v>
       </c>
@@ -1528,7 +1538,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:5">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C47" t="s">
         <v>2</v>
       </c>
@@ -1537,7 +1547,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:5">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
       <c r="C48" t="s">
         <v>3</v>
       </c>
@@ -1546,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="3:4">
+    <row r="49" spans="3:4" x14ac:dyDescent="0.15">
       <c r="C49" t="s">
         <v>4</v>
       </c>
@@ -1556,14 +1566,8 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="1" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>